<commit_message>
added table to parameters
</commit_message>
<xml_diff>
--- a/parameters.xlsx
+++ b/parameters.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\orrzz\Documents\PowerPlantSim\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EF2D0C05-A1CF-484C-81FD-545D7BF2EF39}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3993F907-B7CC-403D-BDEE-7EEEA0AA81DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="32460" yWindow="1545" windowWidth="21600" windowHeight="11295" xr2:uid="{A5523FE8-82CE-4389-86C3-6DFC00E785D2}"/>
+    <workbookView xWindow="38280" yWindow="-120" windowWidth="38640" windowHeight="21120" xr2:uid="{A5523FE8-82CE-4389-86C3-6DFC00E785D2}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="9" uniqueCount="9">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>wh_pressure</t>
   </si>
@@ -63,6 +63,15 @@
   </si>
   <si>
     <t>kg/s</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Column2</t>
+  </si>
+  <si>
+    <t>Parameter</t>
   </si>
 </sst>
 </file>
@@ -115,6 +124,20 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{17033A97-121E-45C3-97F9-CC9742E34F4F}" name="Table1" displayName="Table1" ref="F6:J29" totalsRowShown="0">
+  <autoFilter ref="F6:J29" xr:uid="{17033A97-121E-45C3-97F9-CC9742E34F4F}"/>
+  <tableColumns count="5">
+    <tableColumn id="1" xr3:uid="{E017F47C-CB8E-4033-9A0D-B67C919DA348}" name="Parameter"/>
+    <tableColumn id="2" xr3:uid="{0FAF5C9A-EFAC-4039-8A44-9A92BE2ABC15}" name="V1"/>
+    <tableColumn id="3" xr3:uid="{F764FFD2-7854-448C-855B-727530D4E333}" name="V2"/>
+    <tableColumn id="4" xr3:uid="{AFEC79B0-8E92-440E-A319-500BB78062BB}" name="Total"/>
+    <tableColumn id="5" xr3:uid="{EEB0D398-5460-47E9-A2A6-728C1532E898}" name="Column2"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -436,21 +459,31 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{105E6343-F651-48E8-BAAA-0CA7EFFC5C2E}">
   <dimension ref="F6:J11"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B17" sqref="B17"/>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="D14" sqref="D14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="6" max="6" width="31.42578125" customWidth="1"/>
+    <col min="10" max="10" width="10.28515625" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="6" spans="6:10" x14ac:dyDescent="0.25">
+      <c r="F6" t="s">
+        <v>11</v>
+      </c>
       <c r="G6" t="s">
         <v>6</v>
       </c>
       <c r="H6" t="s">
         <v>7</v>
+      </c>
+      <c r="I6" t="s">
+        <v>9</v>
+      </c>
+      <c r="J6" t="s">
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="6:10" x14ac:dyDescent="0.25">
@@ -500,5 +533,8 @@
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>